<commit_message>
implement testcases chat and call
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>uid</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t>uid_3</t>
+  </si>
+  <si>
+    <t>tutna3</t>
+  </si>
+  <si>
+    <t>uid_4</t>
   </si>
   <si>
     <t>invalid user</t>
@@ -684,8 +690,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1221,13 +1230,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="3" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="4" outlineLevelCol="3"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -1267,7 +1276,7 @@
       <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1276,16 +1285,34 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s">
-        <v>13</v>
+      <c r="D5" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" display="def@456"/>
+    <hyperlink ref="D4" r:id="rId1" display="def@456"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>